<commit_message>
add atoms and bounds
</commit_message>
<xml_diff>
--- a/Manuscript/Standard-bond-energies.xlsx
+++ b/Manuscript/Standard-bond-energies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="114">
   <si>
     <t>Single Bonds</t>
   </si>
@@ -553,6 +553,102 @@
   </si>
   <si>
     <t>Bonds</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>bounds.n</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>atom1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>atom2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Si</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cl</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Br</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CO</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -700,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -715,6 +811,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1048,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1574,596 +1676,1204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.75" customWidth="1"/>
+    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>104.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>38.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2">
         <v>36.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="2">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="2">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="2">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="2">
         <v>93</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="2">
         <v>111</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="2">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="2">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B18" s="2">
         <v>87.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="2">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="2">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="2">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="2">
         <v>154</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="2">
         <v>123</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="2">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="2">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="2">
         <v>85.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="2">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="2">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="2">
         <v>116</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="7">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="2">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="2">
         <v>94</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B36" s="2">
         <v>83</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B37" s="2">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="7">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="2">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B40" s="2">
         <v>132</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="2">
         <v>86</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="7">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B42" s="2">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B43" s="2">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="7">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B44" s="2">
         <v>65</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B45" s="2">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="7">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="2">
         <v>146</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="7">
+        <v>2</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="2">
         <v>109</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="7">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="2">
         <v>119</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="7">
+        <v>2</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B49" s="2">
         <v>147</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="7">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B50" s="2">
         <v>192</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="7">
+        <v>2</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F50" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B51" s="2">
         <v>177</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="7">
+        <v>2</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F51" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B52" s="2">
         <v>178</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="7">
+        <v>2</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B53" s="2">
         <v>179</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="7">
+        <v>2</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B54" s="2">
         <v>179</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="7">
+        <v>2</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B55" s="2">
         <v>177</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="7">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B56" s="2">
         <v>138</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="7">
+        <v>2</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F56" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B57" s="2">
         <v>143</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="7">
+        <v>2</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F57" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B58" s="2">
         <v>110</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="7">
+        <v>2</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B59" s="2">
         <v>70</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="7">
+        <v>2</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B60" s="2">
         <v>128</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="7">
+        <v>2</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B61" s="2">
         <v>93</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="7">
+        <v>2</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F61" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B62" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="7">
+        <v>2</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="2">
         <v>117</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="7">
+        <v>3</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B64" s="2">
         <v>258</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="7">
+        <v>3</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B65" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="7">
+        <v>3</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B66" s="2">
         <v>226</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="7">
+        <v>3</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B67" s="2">
         <v>213</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="14.25" thickTop="1" x14ac:dyDescent="0.15"/>
+      <c r="C67" s="7">
+        <v>3</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>